<commit_message>
Extraccion datos a JSON
</commit_message>
<xml_diff>
--- a/people_scraper/urlsInvestigadores.xlsx
+++ b/people_scraper/urlsInvestigadores.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="128">
   <si>
     <t>No</t>
   </si>
@@ -296,18 +296,6 @@
     <t>https://scienti.minciencias.gov.co/cvlac/visualizador/generarCurriculoCv.do?cod_rh=0000006114</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <color rgb="FF1155CC"/>
-        <u/>
-      </rPr>
-      <t>https://scienti.minciencias.gov.co/gruplac/jsp/visualiza/visualizagr.jsp?nro=00000000001734</t>
-    </r>
-    <r>
-      <t>4</t>
-    </r>
-  </si>
-  <si>
     <t>https://scienti.minciencias.gov.co/cvlac/visualizador/generarCurriculoCv.do?cod_rh=0000415588</t>
   </si>
   <si>
@@ -344,7 +332,7 @@
     <t>- Nombre</t>
   </si>
   <si>
-    <t>/html[1]/body[1]/div[1]/div[3]/table[1]/tr[2]/td[1]/table[1]/]/tr[3]/td[2]/text()</t>
+    <t>/html[1]/body[1]/div[1]/div[3]/table[1]/tr[2]/td[1]/table[1]/tr[3]/td[2]/text()</t>
   </si>
   <si>
     <t>- Titulo</t>
@@ -414,7 +402,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="8">
+  <fonts count="7">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -443,10 +431,6 @@
       <u/>
       <color rgb="FF0000FF"/>
     </font>
-    <font>
-      <u/>
-      <color rgb="FF0000FF"/>
-    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -468,7 +452,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -491,9 +475,6 @@
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="2" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
   </cellXfs>
@@ -1415,8 +1396,8 @@
       <c r="B50" s="4" t="s">
         <v>93</v>
       </c>
-      <c r="C50" s="8" t="s">
-        <v>94</v>
+      <c r="C50" s="3" t="s">
+        <v>87</v>
       </c>
       <c r="D50" s="2" t="s">
         <v>90</v>
@@ -1427,10 +1408,10 @@
         <v>50.0</v>
       </c>
       <c r="B51" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="C51" s="4" t="s">
         <v>95</v>
-      </c>
-      <c r="C51" s="4" t="s">
-        <v>96</v>
       </c>
       <c r="D51" s="2" t="s">
         <v>90</v>
@@ -1441,10 +1422,10 @@
         <v>51.0</v>
       </c>
       <c r="B52" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="C52" s="4" t="s">
         <v>97</v>
-      </c>
-      <c r="C52" s="4" t="s">
-        <v>98</v>
       </c>
       <c r="D52" s="2" t="s">
         <v>90</v>
@@ -1455,10 +1436,10 @@
         <v>52.0</v>
       </c>
       <c r="B53" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="C53" s="4" t="s">
         <v>99</v>
-      </c>
-      <c r="C53" s="4" t="s">
-        <v>100</v>
       </c>
       <c r="D53" s="2" t="s">
         <v>90</v>
@@ -1469,10 +1450,10 @@
         <v>53.0</v>
       </c>
       <c r="B54" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="C54" s="4" t="s">
         <v>101</v>
-      </c>
-      <c r="C54" s="4" t="s">
-        <v>102</v>
       </c>
       <c r="D54" s="2" t="s">
         <v>90</v>
@@ -1483,7 +1464,7 @@
         <v>54.0</v>
       </c>
       <c r="B55" s="4" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C55" s="2" t="s">
         <v>19</v>
@@ -1497,7 +1478,7 @@
         <v>55.0</v>
       </c>
       <c r="B56" s="3" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C56" s="2" t="s">
         <v>19</v>
@@ -1619,112 +1600,112 @@
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
   <cols>
     <col customWidth="1" min="1" max="1" width="32.71"/>
-    <col customWidth="1" min="2" max="2" width="91.71"/>
+    <col customWidth="1" min="2" max="2" width="80.0"/>
   </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="B2" s="6" t="s">
         <v>106</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>107</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="B3" s="6" t="s">
         <v>108</v>
-      </c>
-      <c r="B3" s="6" t="s">
-        <v>109</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="6" t="s">
+        <v>109</v>
+      </c>
+      <c r="B4" s="6" t="s">
         <v>110</v>
-      </c>
-      <c r="B4" s="6" t="s">
-        <v>111</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="B6" s="6" t="s">
         <v>113</v>
-      </c>
-      <c r="B6" s="6" t="s">
-        <v>114</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="B7" s="6" t="s">
         <v>115</v>
-      </c>
-      <c r="B7" s="6" t="s">
-        <v>116</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="B8" s="2" t="s">
         <v>117</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>118</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="2" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="2" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="B14" s="6" t="s">
         <v>123</v>
-      </c>
-      <c r="B14" s="6" t="s">
-        <v>124</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="B15" s="6" t="s">
         <v>125</v>
-      </c>
-      <c r="B15" s="6" t="s">
-        <v>126</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="B16" s="6" t="s">
         <v>127</v>
-      </c>
-      <c r="B16" s="6" t="s">
-        <v>128</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Extraccion de datos de gruplac
</commit_message>
<xml_diff>
--- a/people_scraper/urlsInvestigadores.xlsx
+++ b/people_scraper/urlsInvestigadores.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="126">
   <si>
     <t>No</t>
   </si>
@@ -63,9 +63,6 @@
   </si>
   <si>
     <t>https://scienti.minciencias.gov.co/cvlac/visualizador/generarCurriculoCv.do?cod_rh=0000149616</t>
-  </si>
-  <si>
-    <t>-</t>
   </si>
   <si>
     <t>https://scienti.minciencias.gov.co/cvlac/visualizador/generarCurriculoCv.do?cod_rh=0000906000</t>
@@ -399,7 +396,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="9">
+  <fonts count="11">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -419,11 +416,18 @@
     </font>
     <font>
       <u/>
+      <color rgb="FF0000FF"/>
+    </font>
+    <font>
+      <u/>
       <sz val="11.0"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
     </font>
-    <font/>
+    <font>
+      <u/>
+      <color rgb="FF1155CC"/>
+    </font>
     <font>
       <color rgb="FF000000"/>
     </font>
@@ -435,13 +439,20 @@
       <u/>
       <color rgb="FF0000FF"/>
     </font>
+    <font/>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="lightGray"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor rgb="FFFFFF00"/>
+      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -456,7 +467,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="12">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -469,22 +480,28 @@
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="2" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="2" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="2" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="3" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
   </cellXfs>
@@ -709,7 +726,7 @@
   <cols>
     <col customWidth="1" min="1" max="1" width="9.0"/>
     <col customWidth="1" min="2" max="2" width="102.57"/>
-    <col customWidth="1" min="3" max="3" width="78.43"/>
+    <col customWidth="1" min="3" max="3" width="95.14"/>
     <col customWidth="1" min="4" max="4" width="19.29"/>
   </cols>
   <sheetData>
@@ -745,7 +762,7 @@
       <c r="A3" s="2">
         <v>2.0</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="5" t="s">
         <v>7</v>
       </c>
       <c r="C3" s="4" t="s">
@@ -759,7 +776,7 @@
       <c r="A4" s="2">
         <v>3.0</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="B4" s="6" t="s">
         <v>9</v>
       </c>
       <c r="C4" s="3" t="s">
@@ -773,13 +790,13 @@
       <c r="A5" s="2">
         <v>4.0</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="B5" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="C5" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="D5" s="6" t="s">
+      <c r="D5" s="2" t="s">
         <v>13</v>
       </c>
     </row>
@@ -790,7 +807,7 @@
       <c r="B6" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="C6" s="7" t="s">
         <v>15</v>
       </c>
       <c r="D6" s="2" t="s">
@@ -804,9 +821,7 @@
       <c r="B7" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="C7" s="7" t="s">
-        <v>17</v>
-      </c>
+      <c r="C7" s="8"/>
       <c r="D7" s="2" t="s">
         <v>13</v>
       </c>
@@ -816,9 +831,6 @@
         <v>7.0</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="C8" s="2" t="s">
         <v>17</v>
       </c>
       <c r="D8" s="2" t="s">
@@ -830,10 +842,10 @@
         <v>8.0</v>
       </c>
       <c r="B9" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C9" s="7" t="s">
         <v>19</v>
-      </c>
-      <c r="C9" s="3" t="s">
-        <v>20</v>
       </c>
       <c r="D9" s="2" t="s">
         <v>13</v>
@@ -844,10 +856,10 @@
         <v>9.0</v>
       </c>
       <c r="B10" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C10" s="7" t="s">
         <v>21</v>
-      </c>
-      <c r="C10" s="3" t="s">
-        <v>22</v>
       </c>
       <c r="D10" s="2" t="s">
         <v>13</v>
@@ -858,13 +870,13 @@
         <v>10.0</v>
       </c>
       <c r="B11" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C11" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="C11" s="3" t="s">
-        <v>24</v>
-      </c>
       <c r="D11" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="12">
@@ -872,13 +884,13 @@
         <v>11.0</v>
       </c>
       <c r="B12" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C12" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="C12" s="3" t="s">
-        <v>27</v>
-      </c>
       <c r="D12" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="13">
@@ -886,27 +898,27 @@
         <v>12.0</v>
       </c>
       <c r="B13" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C13" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="C13" s="3" t="s">
-        <v>29</v>
-      </c>
       <c r="D13" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="2">
         <v>13.0</v>
       </c>
-      <c r="B14" s="8" t="s">
+      <c r="B14" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="C14" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="C14" s="3" t="s">
-        <v>31</v>
-      </c>
       <c r="D14" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="15">
@@ -914,13 +926,13 @@
         <v>14.0</v>
       </c>
       <c r="B15" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="C15" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="C15" s="3" t="s">
-        <v>33</v>
-      </c>
       <c r="D15" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="16">
@@ -928,13 +940,10 @@
         <v>15.0</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="C16" s="2" t="s">
-        <v>17</v>
+        <v>33</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="17">
@@ -942,13 +951,13 @@
         <v>16.0</v>
       </c>
       <c r="B17" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C17" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="C17" s="3" t="s">
-        <v>36</v>
-      </c>
       <c r="D17" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="18">
@@ -956,13 +965,13 @@
         <v>17.0</v>
       </c>
       <c r="B18" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="C18" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="C18" s="3" t="s">
-        <v>38</v>
-      </c>
       <c r="D18" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="19">
@@ -970,13 +979,13 @@
         <v>18.0</v>
       </c>
       <c r="B19" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C19" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="C19" s="3" t="s">
-        <v>40</v>
-      </c>
       <c r="D19" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="20">
@@ -984,13 +993,10 @@
         <v>19.0</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="C20" s="2" t="s">
-        <v>17</v>
+        <v>40</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="21">
@@ -998,13 +1004,13 @@
         <v>20.0</v>
       </c>
       <c r="B21" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="C21" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="C21" s="3" t="s">
-        <v>43</v>
-      </c>
       <c r="D21" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="22">
@@ -1012,13 +1018,10 @@
         <v>21.0</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="C22" s="2" t="s">
-        <v>17</v>
+        <v>43</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="23">
@@ -1026,13 +1029,13 @@
         <v>22.0</v>
       </c>
       <c r="B23" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="C23" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="C23" s="3" t="s">
-        <v>46</v>
-      </c>
       <c r="D23" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="24">
@@ -1040,27 +1043,27 @@
         <v>23.0</v>
       </c>
       <c r="B24" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="C24" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="C24" s="3" t="s">
-        <v>48</v>
-      </c>
       <c r="D24" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="2">
         <v>24.0</v>
       </c>
-      <c r="B25" s="9" t="s">
+      <c r="B25" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="C25" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="C25" s="3" t="s">
-        <v>50</v>
-      </c>
       <c r="D25" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="26">
@@ -1068,13 +1071,13 @@
         <v>25.0</v>
       </c>
       <c r="B26" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="C26" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="C26" s="4" t="s">
-        <v>52</v>
-      </c>
       <c r="D26" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="27">
@@ -1082,13 +1085,13 @@
         <v>26.0</v>
       </c>
       <c r="B27" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="C27" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="C27" s="3" t="s">
-        <v>54</v>
-      </c>
       <c r="D27" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="28">
@@ -1096,13 +1099,10 @@
         <v>27.0</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="C28" s="2" t="s">
-        <v>17</v>
+        <v>54</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="29">
@@ -1110,13 +1110,10 @@
         <v>28.0</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="C29" s="2" t="s">
-        <v>17</v>
+        <v>55</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="30">
@@ -1124,69 +1121,63 @@
         <v>29.0</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="C30" s="2" t="s">
-        <v>17</v>
+        <v>56</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="2">
         <v>30.0</v>
       </c>
-      <c r="B31" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="C31" s="2" t="s">
-        <v>17</v>
+      <c r="B31" s="5" t="s">
+        <v>57</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="2">
         <v>31.0</v>
       </c>
-      <c r="B32" s="4" t="s">
+      <c r="B32" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="C32" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="C32" s="4" t="s">
-        <v>60</v>
-      </c>
       <c r="D32" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="2">
         <v>32.0</v>
       </c>
-      <c r="B33" s="4" t="s">
+      <c r="B33" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="C33" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="C33" s="4" t="s">
-        <v>62</v>
-      </c>
       <c r="D33" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="2">
         <v>33.0</v>
       </c>
-      <c r="B34" s="4" t="s">
+      <c r="B34" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="C34" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="C34" s="4" t="s">
-        <v>64</v>
-      </c>
       <c r="D34" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="35">
@@ -1194,27 +1185,24 @@
         <v>34.0</v>
       </c>
       <c r="B35" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="C35" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="C35" s="4" t="s">
-        <v>66</v>
-      </c>
       <c r="D35" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="2">
         <v>35.0</v>
       </c>
-      <c r="B36" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="C36" s="6" t="s">
-        <v>17</v>
+      <c r="B36" s="5" t="s">
+        <v>66</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="37">
@@ -1222,13 +1210,13 @@
         <v>36.0</v>
       </c>
       <c r="B37" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="C37" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="C37" s="4" t="s">
-        <v>69</v>
-      </c>
       <c r="D37" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="38">
@@ -1236,13 +1224,10 @@
         <v>37.0</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="C38" s="6" t="s">
-        <v>17</v>
+        <v>69</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="39">
@@ -1250,27 +1235,21 @@
         <v>38.0</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="C39" s="6" t="s">
-        <v>17</v>
+        <v>70</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" s="2">
         <v>39.0</v>
       </c>
-      <c r="B40" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="C40" s="6" t="s">
-        <v>17</v>
+      <c r="B40" s="5" t="s">
+        <v>71</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="41">
@@ -1278,13 +1257,13 @@
         <v>40.0</v>
       </c>
       <c r="B41" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="C41" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="C41" s="4" t="s">
+      <c r="D41" s="2" t="s">
         <v>74</v>
-      </c>
-      <c r="D41" s="2" t="s">
-        <v>75</v>
       </c>
     </row>
     <row r="42">
@@ -1292,27 +1271,27 @@
         <v>41.0</v>
       </c>
       <c r="B42" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="C42" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="C42" s="4" t="s">
-        <v>77</v>
-      </c>
       <c r="D42" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" s="2">
         <v>42.0</v>
       </c>
-      <c r="B43" s="4" t="s">
+      <c r="B43" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="C43" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="C43" s="4" t="s">
-        <v>79</v>
-      </c>
       <c r="D43" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="44">
@@ -1320,27 +1299,24 @@
         <v>43.0</v>
       </c>
       <c r="B44" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="C44" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="C44" s="4" t="s">
-        <v>81</v>
-      </c>
       <c r="D44" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" s="2">
         <v>44.0</v>
       </c>
-      <c r="B45" s="4" t="s">
-        <v>82</v>
-      </c>
-      <c r="C45" s="6" t="s">
-        <v>17</v>
+      <c r="B45" s="5" t="s">
+        <v>81</v>
       </c>
       <c r="D45" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="46">
@@ -1348,27 +1324,27 @@
         <v>45.0</v>
       </c>
       <c r="B46" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="C46" s="7" t="s">
         <v>83</v>
       </c>
-      <c r="C46" s="4" t="s">
-        <v>84</v>
-      </c>
       <c r="D46" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" s="2">
         <v>46.0</v>
       </c>
-      <c r="B47" s="4" t="s">
+      <c r="B47" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="C47" s="7" t="s">
         <v>85</v>
       </c>
-      <c r="C47" s="3" t="s">
-        <v>86</v>
-      </c>
       <c r="D47" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="48">
@@ -1376,13 +1352,13 @@
         <v>47.0</v>
       </c>
       <c r="B48" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="C48" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="C48" s="4" t="s">
+      <c r="D48" s="2" t="s">
         <v>88</v>
-      </c>
-      <c r="D48" s="2" t="s">
-        <v>89</v>
       </c>
     </row>
     <row r="49">
@@ -1390,41 +1366,41 @@
         <v>48.0</v>
       </c>
       <c r="B49" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="C49" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="C49" s="4" t="s">
-        <v>91</v>
-      </c>
       <c r="D49" s="2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" s="2">
         <v>49.0</v>
       </c>
-      <c r="B50" s="4" t="s">
-        <v>92</v>
+      <c r="B50" s="5" t="s">
+        <v>91</v>
       </c>
       <c r="C50" s="3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D50" s="2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" s="2">
         <v>50.0</v>
       </c>
-      <c r="B51" s="4" t="s">
+      <c r="B51" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="C51" s="3" t="s">
         <v>93</v>
       </c>
-      <c r="C51" s="4" t="s">
-        <v>94</v>
-      </c>
       <c r="D51" s="2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="52">
@@ -1432,55 +1408,52 @@
         <v>51.0</v>
       </c>
       <c r="B52" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="C52" s="4" t="s">
         <v>95</v>
       </c>
-      <c r="C52" s="4" t="s">
-        <v>96</v>
-      </c>
       <c r="D52" s="2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" s="2">
         <v>52.0</v>
       </c>
-      <c r="B53" s="4" t="s">
+      <c r="B53" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="C53" s="4" t="s">
         <v>97</v>
       </c>
-      <c r="C53" s="4" t="s">
-        <v>98</v>
-      </c>
       <c r="D53" s="2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" s="2">
         <v>53.0</v>
       </c>
-      <c r="B54" s="4" t="s">
+      <c r="B54" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="C54" s="4" t="s">
         <v>99</v>
       </c>
-      <c r="C54" s="4" t="s">
-        <v>100</v>
-      </c>
       <c r="D54" s="2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" s="2">
         <v>54.0</v>
       </c>
-      <c r="B55" s="4" t="s">
-        <v>101</v>
-      </c>
-      <c r="C55" s="2" t="s">
-        <v>17</v>
+      <c r="B55" s="5" t="s">
+        <v>100</v>
       </c>
       <c r="D55" s="2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="56">
@@ -1488,13 +1461,10 @@
         <v>55.0</v>
       </c>
       <c r="B56" s="3" t="s">
-        <v>102</v>
-      </c>
-      <c r="C56" s="2" t="s">
-        <v>17</v>
+        <v>101</v>
       </c>
       <c r="D56" s="2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
   </sheetData>
@@ -1614,107 +1584,107 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="B2" s="11" t="s">
         <v>104</v>
-      </c>
-      <c r="B2" s="6" t="s">
-        <v>105</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="B3" s="11" t="s">
         <v>106</v>
       </c>
-      <c r="B3" s="6" t="s">
+    </row>
+    <row r="4">
+      <c r="A4" s="11" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="6" t="s">
+      <c r="B4" s="11" t="s">
         <v>108</v>
-      </c>
-      <c r="B4" s="6" t="s">
-        <v>109</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="2" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="B6" s="11" t="s">
         <v>111</v>
-      </c>
-      <c r="B6" s="6" t="s">
-        <v>112</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="B7" s="11" t="s">
         <v>113</v>
-      </c>
-      <c r="B7" s="6" t="s">
-        <v>114</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="B8" s="2" t="s">
         <v>115</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>116</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="2" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="B11" s="6" t="s">
-        <v>118</v>
+        <v>103</v>
+      </c>
+      <c r="B11" s="11" t="s">
+        <v>117</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="B14" s="11" t="s">
         <v>121</v>
-      </c>
-      <c r="B14" s="6" t="s">
-        <v>122</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="B15" s="11" t="s">
         <v>123</v>
-      </c>
-      <c r="B15" s="6" t="s">
-        <v>124</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="B16" s="11" t="s">
         <v>125</v>
-      </c>
-      <c r="B16" s="6" t="s">
-        <v>126</v>
       </c>
     </row>
   </sheetData>

</xml_diff>